<commit_message>
support for multi-sheet excel files
</commit_message>
<xml_diff>
--- a/utilities/resources/workloads-import-example.xlsx
+++ b/utilities/resources/workloads-import-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://illumio-my.sharepoint.com/personal/christophe_painchaud_illumio_com/Documents/Synced/dev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://illumio-my.sharepoint.com/personal/christophe_painchaud_illumio_com/Documents/Synced/dev/pylo/utilities/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63639AB7-BB7A-44F0-8117-10C69E46CEA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{63639AB7-BB7A-44F0-8117-10C69E46CEA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A5A6E8C0-93DD-42CE-B992-703D38B475BC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workloads-import-example" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,12 +901,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -960,6 +963,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFBED304A129CC4EB3EB3F3612692590" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e55902cb5f207ba6533a7cbfc2b422e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="418c3449-820c-4050-a2e7-95db9dcc5f30" xmlns:ns4="0d03ce2c-e80a-41bc-84d7-9f741c2b71ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3bdee3454a96eb7015338206f810d20" ns3:_="" ns4:_="">
     <xsd:import namespace="418c3449-820c-4050-a2e7-95db9dcc5f30"/>
@@ -1144,22 +1162,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADEC72C-EABA-4F21-8AB5-D28D9F66DD55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="0d03ce2c-e80a-41bc-84d7-9f741c2b71ce"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="418c3449-820c-4050-a2e7-95db9dcc5f30"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BCE2EF6-CDA4-4AD0-A42E-3237585D256E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{678CC710-2B9C-48FD-A1E6-CD8C23C23493}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1176,29 +1204,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BCE2EF6-CDA4-4AD0-A42E-3237585D256E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADEC72C-EABA-4F21-8AB5-D28D9F66DD55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0d03ce2c-e80a-41bc-84d7-9f741c2b71ce"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="418c3449-820c-4050-a2e7-95db9dcc5f30"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>